<commit_message>
StackItem Count 출력 추가
</commit_message>
<xml_diff>
--- a/Document/Data/Effect/Effect.xlsx
+++ b/Document/Data/Effect/Effect.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HavePoop\Desktop\Study\Core\Document\Data\Effect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468B18A9-58D7-43C4-BA08-52FF8F203A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4029EC-27A1-4C07-A9D0-17B53D7CA8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17010" yWindow="4365" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ability" sheetId="12" r:id="rId1"/>
+    <sheet name="Effect" sheetId="12" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -475,7 +475,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>